<commit_message>
Update 2020-03-16: including US again.
</commit_message>
<xml_diff>
--- a/covid-manual-excel.xlsx
+++ b/covid-manual-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspaces\covid-19-data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499DFF6-545A-4EB0-B900-F75FDA9C2A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544CFEB5-6722-4CFD-813E-38591E23D151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="18960" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="18960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Italy" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="France" sheetId="2" r:id="rId3"/>
     <sheet name="Spain" sheetId="3" r:id="rId4"/>
     <sheet name="United Kingdom" sheetId="4" r:id="rId5"/>
-    <sheet name="United States" sheetId="7" r:id="rId6"/>
+    <sheet name="US" sheetId="7" r:id="rId6"/>
     <sheet name="Austria" sheetId="8" r:id="rId7"/>
     <sheet name="Switzerland" sheetId="9" r:id="rId8"/>
     <sheet name="Korea, South" sheetId="11" r:id="rId9"/>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E75EBFD-15CF-4FAD-9CA9-0C1E4CDC9AF7}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +457,20 @@
         <v>1441</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>24747</v>
+      </c>
+      <c r="C5">
+        <v>2335</v>
+      </c>
+      <c r="D5">
+        <v>1809</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -465,10 +479,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DB2288-E66E-44BC-933C-9471E73C5145}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +546,20 @@
       </c>
       <c r="D4">
         <v>611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>13938</v>
+      </c>
+      <c r="C5">
+        <v>4590</v>
+      </c>
+      <c r="D5">
+        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -577,10 +605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +674,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>5813</v>
+      </c>
+      <c r="C5">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -654,10 +696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584CF58A-B6AB-4B55-A232-0ECA8145474E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +765,20 @@
         <v>91</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>5423</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -731,10 +787,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526A6C31-C389-4FCA-ABC1-1A7A35286209}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,6 +856,20 @@
         <v>196</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>7844</v>
+      </c>
+      <c r="C5">
+        <v>517</v>
+      </c>
+      <c r="D5">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -808,10 +878,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCED248-DC47-4D72-B4A8-11B0E4326564}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,6 +947,23 @@
         <v>21</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>1372</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -885,10 +972,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DAB03D-2093-43D6-930A-C5C263DB0B65}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,6 +1041,20 @@
         <v>57</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>3791</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -962,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8DAF25-F5B0-47E4-BAFA-42517715F0C0}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1132,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>860</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1039,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93D820-3EC4-4C78-B8BB-92CDAF853513}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,6 +1223,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>2200</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1116,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E279C389-C415-4B73-9113-FDA48BBDF828}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,6 +1314,20 @@
         <v>75</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43906.337500000001</v>
+      </c>
+      <c r="B5">
+        <v>8236</v>
+      </c>
+      <c r="C5">
+        <v>1137</v>
+      </c>
+      <c r="D5">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>